<commit_message>
May 27 Update after discussion with Anshika
no defect list replaced
presentation updated
new report generated
PV hours report generated till april
</commit_message>
<xml_diff>
--- a/Defect list/SPRF with no defect.xlsx
+++ b/Defect list/SPRF with no defect.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$J$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,7 +32,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -41,7 +41,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Gulani Gurpreet was QCA lead</t>
@@ -56,7 +56,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -65,7 +65,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 As per Sashi Test only Project</t>
@@ -80,7 +80,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -89,7 +89,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Yeraballi and Gurpreet from QCA side and Ashwini from dev side, UHN reporting</t>
@@ -104,7 +104,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -113,7 +113,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Hameed was QCA lead, Dev was Gabe Enabore</t>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>Sprf Name</t>
   </si>
@@ -260,6 +260,39 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>This was moved to Q3_Int_2012 and has 113 Defects</t>
+  </si>
+  <si>
+    <t>Nothin in Adr for Q1_int. As per ADR this is a 2011-11 project</t>
+  </si>
+  <si>
+    <t>No Defects</t>
+  </si>
+  <si>
+    <t>Nothin in ADR for Q2_Non_Int_2012. As per ADR this is a 2011 project</t>
+  </si>
+  <si>
+    <t>As per adr this is a Q3 2012 project. Has 58 Defects in Q3 2012 in QC</t>
+  </si>
+  <si>
+    <t>Nothing in Q3-2012</t>
+  </si>
+  <si>
+    <t>Cannot validate. Instance Migrated from QC and not yet available in ALM</t>
+  </si>
+  <si>
+    <t>Cannot Validate. Instance migrated from QC and not available in ALM yet</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Nothing in adr for 2012</t>
+  </si>
+  <si>
+    <t>Total Defect</t>
   </si>
 </sst>
 </file>
@@ -303,17 +336,17 @@
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +356,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,6 +405,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I32"/>
+  <dimension ref="B2:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,12 +723,14 @@
     <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>43</v>
       </c>
@@ -696,20 +743,23 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -722,12 +772,17 @@
       <c r="E3" s="4">
         <v>1720</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="8">
+        <v>113</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -740,12 +795,15 @@
       <c r="E4" s="4">
         <v>1480</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -758,12 +816,17 @@
       <c r="E5" s="4">
         <v>1302.5</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -776,12 +839,15 @@
       <c r="E6" s="4">
         <v>1291.5</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -794,12 +860,17 @@
       <c r="E7" s="4">
         <v>1046.5</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -812,12 +883,17 @@
       <c r="E8" s="4">
         <v>983</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -830,12 +906,17 @@
       <c r="E9" s="4">
         <v>855.25</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -848,12 +929,17 @@
       <c r="E10" s="4">
         <v>784.5</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -866,12 +952,15 @@
       <c r="E11" s="4">
         <v>729</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -884,12 +973,15 @@
       <c r="E12" s="4">
         <v>696.25</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -902,12 +994,15 @@
       <c r="E13" s="4">
         <v>684.25</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>12</v>
       </c>
@@ -920,12 +1015,17 @@
       <c r="E14" s="4">
         <v>627</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>13</v>
       </c>
@@ -938,12 +1038,15 @@
       <c r="E15" s="4">
         <v>608.25</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>14</v>
       </c>
@@ -956,12 +1059,17 @@
       <c r="E16" s="4">
         <v>585.25</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>15</v>
       </c>
@@ -974,16 +1082,21 @@
       <c r="E17" s="4">
         <v>567.5</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -992,12 +1105,17 @@
       <c r="E18" s="4">
         <v>546.5</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>17</v>
       </c>
@@ -1010,14 +1128,19 @@
       <c r="E19" s="4">
         <v>477</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="8">
         <v>14</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5">
+        <v>14</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>18</v>
       </c>
@@ -1030,12 +1153,17 @@
       <c r="E20" s="4">
         <v>458.5</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>19</v>
       </c>
@@ -1048,12 +1176,15 @@
       <c r="E21" s="4">
         <v>445.25</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
         <v>20</v>
       </c>
@@ -1066,12 +1197,17 @@
       <c r="E22" s="4">
         <v>402</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>21</v>
       </c>
@@ -1084,12 +1220,15 @@
       <c r="E23" s="4">
         <v>378.25</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
         <v>22</v>
       </c>
@@ -1102,12 +1241,17 @@
       <c r="E24" s="4">
         <v>375</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="8">
+        <v>0</v>
+      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>23</v>
       </c>
@@ -1120,12 +1264,15 @@
       <c r="E25" s="4">
         <v>370.25</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>24</v>
       </c>
@@ -1138,12 +1285,15 @@
       <c r="E26" s="4">
         <v>303.25</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>25</v>
       </c>
@@ -1156,12 +1306,15 @@
       <c r="E27" s="4">
         <v>281.75</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="8"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>26</v>
       </c>
@@ -1174,12 +1327,17 @@
       <c r="E28" s="4">
         <v>272.75</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="8">
+        <v>58</v>
+      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>27</v>
       </c>
@@ -1192,14 +1350,19 @@
       <c r="E29" s="4">
         <v>259.5</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="8">
         <v>94</v>
       </c>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5">
+        <v>94</v>
+      </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>28</v>
       </c>
@@ -1212,12 +1375,15 @@
       <c r="E30" s="4">
         <v>251.5</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>29</v>
       </c>
@@ -1230,12 +1396,15 @@
       <c r="E31" s="4">
         <v>218.5</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>30</v>
       </c>
@@ -1248,15 +1417,20 @@
       <c r="E32" s="4">
         <v>121.75</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="8">
+        <v>0</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
+      <c r="J32" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:H2">
-    <sortState ref="C3:H32">
-      <sortCondition descending="1" ref="E2"/>
+  <autoFilter ref="B2:J32">
+    <sortState ref="B3:I32">
+      <sortCondition descending="1" ref="E2:E32"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>